<commit_message>
Fixed Internal factions, minor file changes
</commit_message>
<xml_diff>
--- a/Modding resources/Internal Factions Completed.xlsx
+++ b/Modding resources/Internal Factions Completed.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HoChiMinh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HoChiMinh/Documents/Paradox Interactive/Hearts of Iron IV/mod/Modern_Day_4_HOI/Modding resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -63,6 +63,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2004,11 +2005,6 @@
     <t>PKK</t>
   </si>
   <si>
-    <t>MIL
-FRM
-SSBM</t>
-  </si>
-  <si>
     <t>Polynesian Federation</t>
   </si>
   <si>
@@ -2095,11 +2091,6 @@
   </si>
   <si>
     <t>ROJ</t>
-  </si>
-  <si>
-    <t>FRM
-MIL
-FJI</t>
   </si>
   <si>
     <t>Romania</t>
@@ -2864,12 +2855,23 @@
 countries
 </t>
   </si>
+  <si>
+    <t>MIL
+FRM
+LAU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRM
+MIL
+NTL
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2915,6 +2917,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -3279,7 +3287,7 @@
   <dimension ref="A1:F1046"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E189" sqref="E189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3295,10 +3303,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3323,10 +3331,10 @@
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
@@ -5679,8 +5687,8 @@
       <c r="B176" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="C176" s="3" t="s">
-        <v>525</v>
+      <c r="C176" s="7" t="s">
+        <v>756</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>65</v>
@@ -5688,13 +5696,13 @@
     </row>
     <row r="177" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="B177" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="B177" s="3" t="s">
+      <c r="C177" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>528</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>65</v>
@@ -5702,37 +5710,37 @@
     </row>
     <row r="178" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="B178" s="3" t="s">
         <v>529</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>530</v>
       </c>
       <c r="C178" s="3"/>
       <c r="D178" s="3"/>
     </row>
     <row r="179" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
+        <v>530</v>
+      </c>
+      <c r="B179" t="s">
         <v>531</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C179" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="C179" s="3" t="s">
+      <c r="D179" s="3" t="s">
         <v>533</v>
-      </c>
-      <c r="D179" s="3" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
+        <v>534</v>
+      </c>
+      <c r="B180" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="B180" s="3" t="s">
+      <c r="C180" s="3" t="s">
         <v>536</v>
-      </c>
-      <c r="C180" s="3" t="s">
-        <v>537</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>113</v>
@@ -5740,23 +5748,23 @@
     </row>
     <row r="181" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B181" s="3" t="s">
         <v>538</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>539</v>
       </c>
       <c r="C181" s="3"/>
       <c r="D181" s="3"/>
     </row>
     <row r="182" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
+        <v>539</v>
+      </c>
+      <c r="B182" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="B182" s="3" t="s">
+      <c r="C182" s="3" t="s">
         <v>541</v>
-      </c>
-      <c r="C182" s="3" t="s">
-        <v>542</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>49</v>
@@ -5764,13 +5772,13 @@
     </row>
     <row r="183" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
+        <v>542</v>
+      </c>
+      <c r="B183" t="s">
         <v>543</v>
       </c>
-      <c r="B183" t="s">
+      <c r="C183" s="3" t="s">
         <v>544</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>545</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>479</v>
@@ -5778,20 +5786,20 @@
     </row>
     <row r="184" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="B184" s="3" t="s">
         <v>546</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>547</v>
       </c>
       <c r="C184" s="3"/>
       <c r="D184" s="3"/>
     </row>
     <row r="185" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>343</v>
@@ -5802,13 +5810,13 @@
     </row>
     <row r="186" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="B186" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="B186" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>551</v>
+      <c r="C186" s="7" t="s">
+        <v>757</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>205</v>
@@ -5816,13 +5824,13 @@
     </row>
     <row r="187" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
+        <v>550</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="C187" s="3" t="s">
         <v>552</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="C187" s="3" t="s">
-        <v>554</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>113</v>
@@ -5830,24 +5838,24 @@
     </row>
     <row r="188" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>553</v>
+      </c>
+      <c r="B188" t="s">
+        <v>554</v>
+      </c>
+      <c r="C188" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="B188" t="s">
+      <c r="D188" s="3" t="s">
         <v>556</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>557</v>
-      </c>
-      <c r="D188" s="3" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>56</v>
@@ -5858,10 +5866,10 @@
     </row>
     <row r="190" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>86</v>
@@ -5872,10 +5880,10 @@
     </row>
     <row r="191" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B191" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>94</v>
@@ -5886,47 +5894,47 @@
     </row>
     <row r="192" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C192" s="3"/>
       <c r="D192" s="3"/>
     </row>
     <row r="193" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C193" s="3"/>
       <c r="D193" s="3"/>
     </row>
     <row r="194" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="C194" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="B194" s="3" t="s">
+      <c r="D194" s="3" t="s">
         <v>570</v>
-      </c>
-      <c r="C194" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="D194" s="3" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
+        <v>571</v>
+      </c>
+      <c r="B195" t="s">
+        <v>572</v>
+      </c>
+      <c r="C195" s="3" t="s">
         <v>573</v>
-      </c>
-      <c r="B195" t="s">
-        <v>574</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>575</v>
       </c>
       <c r="D195" s="3" t="s">
         <v>407</v>
@@ -5934,10 +5942,10 @@
     </row>
     <row r="196" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>452</v>
@@ -5948,13 +5956,13 @@
     </row>
     <row r="197" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>576</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="C197" s="3" t="s">
         <v>578</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>579</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>580</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>238</v>
@@ -5962,86 +5970,86 @@
     </row>
     <row r="198" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="C198" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="B198" s="3" t="s">
+      <c r="D198" s="3" t="s">
         <v>582</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="D198" s="3" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="5" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>352</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="3"/>
     </row>
     <row r="201" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="C201" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="B201" s="3" t="s">
+      <c r="D201" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>592</v>
-      </c>
-      <c r="D201" s="3" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>592</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="C202" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="B202" s="3" t="s">
+      <c r="D202" s="3" t="s">
         <v>595</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>596</v>
-      </c>
-      <c r="D202" s="3" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
     </row>
     <row r="204" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>508</v>
@@ -6052,10 +6060,10 @@
     </row>
     <row r="205" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>201</v>
@@ -6066,10 +6074,10 @@
     </row>
     <row r="206" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>56</v>
@@ -6080,13 +6088,13 @@
     </row>
     <row r="207" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="C207" s="3" t="s">
         <v>606</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>607</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>608</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>407</v>
@@ -6094,13 +6102,13 @@
     </row>
     <row r="208" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="C208" s="3" t="s">
         <v>609</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>610</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>611</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>401</v>
@@ -6108,37 +6116,37 @@
     </row>
     <row r="209" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
+        <v>610</v>
+      </c>
+      <c r="B209" t="s">
+        <v>611</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="D209" s="3" t="s">
         <v>612</v>
-      </c>
-      <c r="B209" t="s">
-        <v>613</v>
-      </c>
-      <c r="C209" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="D209" s="3" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C210" s="3"/>
       <c r="D210" s="3"/>
     </row>
     <row r="211" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="C211" s="3" t="s">
         <v>617</v>
-      </c>
-      <c r="B211" s="3" t="s">
-        <v>618</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>619</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>65</v>
@@ -6146,23 +6154,23 @@
     </row>
     <row r="212" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C212" s="3"/>
       <c r="D212" s="3"/>
     </row>
     <row r="213" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
+        <v>619</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="C213" s="3" t="s">
         <v>621</v>
-      </c>
-      <c r="B213" s="3" t="s">
-        <v>622</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>623</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>273</v>
@@ -6170,13 +6178,13 @@
     </row>
     <row r="214" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="C214" s="3" t="s">
         <v>624</v>
-      </c>
-      <c r="B214" s="3" t="s">
-        <v>625</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>626</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>65</v>
@@ -6184,13 +6192,13 @@
     </row>
     <row r="215" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
+        <v>625</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C215" s="3" t="s">
         <v>627</v>
-      </c>
-      <c r="B215" s="3" t="s">
-        <v>628</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>629</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>53</v>
@@ -6198,13 +6206,13 @@
     </row>
     <row r="216" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
+        <v>628</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="C216" s="3" t="s">
         <v>630</v>
-      </c>
-      <c r="B216" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="C216" s="3" t="s">
-        <v>632</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>445</v>
@@ -6212,23 +6220,23 @@
     </row>
     <row r="217" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C217" s="3"/>
       <c r="D217" s="3"/>
     </row>
     <row r="218" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="C218" s="3" t="s">
         <v>635</v>
-      </c>
-      <c r="B218" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="C218" s="3" t="s">
-        <v>637</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>113</v>
@@ -6236,13 +6244,13 @@
     </row>
     <row r="219" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="C219" s="3" t="s">
         <v>638</v>
-      </c>
-      <c r="B219" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>640</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>95</v>
@@ -6250,38 +6258,38 @@
     </row>
     <row r="220" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="C220" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="B220" s="3" t="s">
+      <c r="D220" s="3" t="s">
         <v>642</v>
-      </c>
-      <c r="C220" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="D220" s="3" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
+        <v>643</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="C221" s="3" t="s">
         <v>645</v>
-      </c>
-      <c r="B221" s="3" t="s">
-        <v>646</v>
-      </c>
-      <c r="C221" s="3" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
+        <v>646</v>
+      </c>
+      <c r="B222" t="s">
+        <v>647</v>
+      </c>
+      <c r="C222" s="3" t="s">
         <v>648</v>
-      </c>
-      <c r="B222" t="s">
-        <v>649</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>650</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>99</v>
@@ -6289,10 +6297,10 @@
     </row>
     <row r="223" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>457</v>
@@ -6303,10 +6311,10 @@
     </row>
     <row r="224" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B224" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>262</v>
@@ -6317,27 +6325,27 @@
     </row>
     <row r="225" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
+        <v>653</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="C225" s="3" t="s">
         <v>655</v>
       </c>
-      <c r="B225" s="3" t="s">
+      <c r="D225" s="3" t="s">
         <v>656</v>
-      </c>
-      <c r="C225" s="3" t="s">
-        <v>657</v>
-      </c>
-      <c r="D225" s="3" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
+        <v>657</v>
+      </c>
+      <c r="B226" t="s">
+        <v>658</v>
+      </c>
+      <c r="C226" s="3" t="s">
         <v>659</v>
-      </c>
-      <c r="B226" t="s">
-        <v>660</v>
-      </c>
-      <c r="C226" s="3" t="s">
-        <v>661</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>65</v>
@@ -6345,34 +6353,34 @@
     </row>
     <row r="227" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="B227" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="C227" s="3" t="s">
         <v>662</v>
       </c>
-      <c r="B227" s="3" t="s">
+      <c r="D227" s="3" t="s">
         <v>663</v>
-      </c>
-      <c r="C227" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="D227" s="3" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C228" s="3"/>
       <c r="D228" s="3"/>
     </row>
     <row r="229" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
+        <v>665</v>
+      </c>
+      <c r="B229" t="s">
+        <v>666</v>
+      </c>
+      <c r="C229" s="3" t="s">
         <v>667</v>
-      </c>
-      <c r="B229" t="s">
-        <v>668</v>
-      </c>
-      <c r="C229" s="3" t="s">
-        <v>669</v>
       </c>
       <c r="D229" s="3" t="s">
         <v>53</v>
@@ -6380,13 +6388,13 @@
     </row>
     <row r="230" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="C230" s="3" t="s">
         <v>670</v>
-      </c>
-      <c r="B230" s="3" t="s">
-        <v>671</v>
-      </c>
-      <c r="C230" s="3" t="s">
-        <v>672</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>65</v>
@@ -6394,33 +6402,33 @@
     </row>
     <row r="231" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C231" s="3"/>
       <c r="D231" s="3"/>
     </row>
     <row r="232" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C232" s="3"/>
       <c r="D232" s="3"/>
     </row>
     <row r="233" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="C233" s="3" t="s">
         <v>677</v>
-      </c>
-      <c r="B233" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="C233" s="3" t="s">
-        <v>679</v>
       </c>
       <c r="D233" s="4" t="s">
         <v>49</v>
@@ -6428,13 +6436,13 @@
     </row>
     <row r="234" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
+        <v>678</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="C234" s="3" t="s">
         <v>680</v>
-      </c>
-      <c r="B234" s="3" t="s">
-        <v>681</v>
-      </c>
-      <c r="C234" s="3" t="s">
-        <v>682</v>
       </c>
       <c r="D234" s="3" t="s">
         <v>139</v>
@@ -6442,10 +6450,10 @@
     </row>
     <row r="235" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C235" s="3" t="s">
         <v>141</v>
@@ -6456,13 +6464,13 @@
     </row>
     <row r="236" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="B236" t="s">
+        <v>684</v>
+      </c>
+      <c r="C236" s="3" t="s">
         <v>685</v>
-      </c>
-      <c r="B236" t="s">
-        <v>686</v>
-      </c>
-      <c r="C236" s="3" t="s">
-        <v>687</v>
       </c>
       <c r="D236" s="3" t="s">
         <v>49</v>
@@ -6470,27 +6478,27 @@
     </row>
     <row r="237" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
+        <v>688</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="C238" s="3" t="s">
         <v>690</v>
-      </c>
-      <c r="B238" s="3" t="s">
-        <v>691</v>
-      </c>
-      <c r="C238" s="3" t="s">
-        <v>692</v>
       </c>
       <c r="D238" s="3" t="s">
         <v>113</v>
@@ -6498,13 +6506,13 @@
     </row>
     <row r="239" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="C239" s="3" t="s">
         <v>693</v>
-      </c>
-      <c r="B239" s="3" t="s">
-        <v>694</v>
-      </c>
-      <c r="C239" s="3" t="s">
-        <v>695</v>
       </c>
       <c r="D239" s="3" t="s">
         <v>65</v>
@@ -6512,27 +6520,27 @@
     </row>
     <row r="240" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>204</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
+        <v>697</v>
+      </c>
+      <c r="B241" t="s">
+        <v>698</v>
+      </c>
+      <c r="C241" s="3" t="s">
         <v>699</v>
-      </c>
-      <c r="B241" t="s">
-        <v>700</v>
-      </c>
-      <c r="C241" s="3" t="s">
-        <v>701</v>
       </c>
       <c r="D241" s="3" t="s">
         <v>113</v>
@@ -6540,13 +6548,13 @@
     </row>
     <row r="242" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="B242" t="s">
+        <v>701</v>
+      </c>
+      <c r="C242" s="3" t="s">
         <v>702</v>
-      </c>
-      <c r="B242" t="s">
-        <v>703</v>
-      </c>
-      <c r="C242" s="3" t="s">
-        <v>704</v>
       </c>
       <c r="D242" s="3" t="s">
         <v>273</v>
@@ -6554,24 +6562,24 @@
     </row>
     <row r="243" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
+        <v>703</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="C243" s="3" t="s">
         <v>705</v>
       </c>
-      <c r="B243" s="3" t="s">
+      <c r="D243" s="3" t="s">
         <v>706</v>
-      </c>
-      <c r="C243" s="3" t="s">
-        <v>707</v>
-      </c>
-      <c r="D243" s="3" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B244" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C244" s="3" t="s">
         <v>303</v>
@@ -6582,13 +6590,13 @@
     </row>
     <row r="245" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="B245" t="s">
+        <v>710</v>
+      </c>
+      <c r="C245" s="3" t="s">
         <v>711</v>
-      </c>
-      <c r="B245" t="s">
-        <v>712</v>
-      </c>
-      <c r="C245" s="3" t="s">
-        <v>713</v>
       </c>
       <c r="D245" s="3" t="s">
         <v>139</v>
@@ -6596,41 +6604,41 @@
     </row>
     <row r="246" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>83</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
+        <v>714</v>
+      </c>
+      <c r="B247" t="s">
+        <v>715</v>
+      </c>
+      <c r="C247" s="3" t="s">
         <v>716</v>
       </c>
-      <c r="B247" t="s">
+      <c r="D247" s="3" t="s">
         <v>717</v>
-      </c>
-      <c r="C247" s="3" t="s">
-        <v>718</v>
-      </c>
-      <c r="D247" s="3" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
+        <v>718</v>
+      </c>
+      <c r="B248" t="s">
+        <v>719</v>
+      </c>
+      <c r="C248" s="3" t="s">
         <v>720</v>
-      </c>
-      <c r="B248" t="s">
-        <v>721</v>
-      </c>
-      <c r="C248" s="3" t="s">
-        <v>722</v>
       </c>
       <c r="D248" s="3" t="s">
         <v>227</v>
@@ -6638,27 +6646,27 @@
     </row>
     <row r="249" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="B249" t="s">
+        <v>722</v>
+      </c>
+      <c r="C249" s="3" t="s">
         <v>723</v>
       </c>
-      <c r="B249" t="s">
+      <c r="D249" s="3" t="s">
         <v>724</v>
-      </c>
-      <c r="C249" s="3" t="s">
-        <v>725</v>
-      </c>
-      <c r="D249" s="3" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="B250" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="C250" s="3" t="s">
         <v>727</v>
-      </c>
-      <c r="B250" s="3" t="s">
-        <v>728</v>
-      </c>
-      <c r="C250" s="3" t="s">
-        <v>729</v>
       </c>
       <c r="D250" s="3" t="s">
         <v>99</v>
@@ -6666,13 +6674,13 @@
     </row>
     <row r="251" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
+        <v>728</v>
+      </c>
+      <c r="B251" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="C251" s="3" t="s">
         <v>730</v>
-      </c>
-      <c r="B251" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="C251" s="3" t="s">
-        <v>732</v>
       </c>
       <c r="D251" s="3" t="s">
         <v>57</v>
@@ -6680,65 +6688,65 @@
     </row>
     <row r="252" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="B252" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="C252" s="3" t="s">
         <v>733</v>
-      </c>
-      <c r="B252" s="3" t="s">
-        <v>734</v>
-      </c>
-      <c r="C252" s="3" t="s">
-        <v>735</v>
       </c>
       <c r="D252" s="3"/>
     </row>
     <row r="253" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="3"/>
     </row>
     <row r="254" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3"/>
     </row>
     <row r="255" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3"/>
     </row>
     <row r="256" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C256" s="3"/>
       <c r="D256" s="3"/>
     </row>
     <row r="257" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B257" t="s">
+        <v>741</v>
+      </c>
+      <c r="C257" s="3" t="s">
         <v>743</v>
-      </c>
-      <c r="C257" s="3" t="s">
-        <v>745</v>
       </c>
       <c r="D257" s="3" t="s">
         <v>380</v>
@@ -6746,28 +6754,28 @@
     </row>
     <row r="258" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C258" s="3"/>
     </row>
     <row r="259" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C259" s="3"/>
     </row>
     <row r="260" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>473</v>
@@ -6778,10 +6786,10 @@
     </row>
     <row r="261" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C261" s="3" t="s">
         <v>98</v>

</xml_diff>